<commit_message>
add sentences and new theme
</commit_message>
<xml_diff>
--- a/appDE.xlsx
+++ b/appDE.xlsx
@@ -22514,7 +22514,7 @@
   <dimension ref="A1:L1580"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1466" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K1479" sqref="K1479"/>
     </sheetView>
   </sheetViews>
@@ -26103,7 +26103,7 @@
         <v>5568</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="s">
         <v>1462</v>
       </c>
@@ -26135,7 +26135,7 @@
         <v>5570</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="9" t="s">
         <v>1461</v>
       </c>
@@ -26167,7 +26167,7 @@
         <v>5572</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="9" t="s">
         <v>1461</v>
       </c>
@@ -26518,7 +26518,7 @@
         <v>5594</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="9" t="s">
         <v>1462</v>
       </c>
@@ -27610,7 +27610,7 @@
         <v>5662</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="9" t="s">
         <v>1462</v>
       </c>
@@ -27642,7 +27642,7 @@
         <v>5664</v>
       </c>
     </row>
-    <row r="167" spans="1:12" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A167" s="9" t="s">
         <v>1462</v>
       </c>
@@ -28531,7 +28531,7 @@
         <v>5722</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A196" s="12" t="s">
         <v>1463</v>
       </c>
@@ -28793,7 +28793,7 @@
         <v>5740</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:12" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A205" s="12" t="s">
         <v>1463</v>
       </c>

</xml_diff>